<commit_message>
dev of dragon buff
</commit_message>
<xml_diff>
--- a/gameData/shared/DragonEquipments.xlsx
+++ b/gameData/shared/DragonEquipments.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3760" yWindow="2460" windowWidth="25600" windowHeight="16060" tabRatio="883"/>
+    <workbookView xWindow="12660" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="883" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="equipments" sheetId="62" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="159">
   <si>
     <t>INT_strength</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -660,6 +660,10 @@
   </si>
   <si>
     <t>ingo_1:1,redCrystal_1:1</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_leadership</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -841,7 +845,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1368">
+  <cellStyleXfs count="1386">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -856,6 +860,24 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2233,7 +2255,7 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1368">
+  <cellStyles count="1386">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -2920,6 +2942,15 @@
     <cellStyle name="超链接" xfId="1362" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="1364" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="1366" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1368" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1370" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1372" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1374" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1376" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1378" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1380" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1382" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1384" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -3599,6 +3630,15 @@
     <cellStyle name="访问过的超链接" xfId="1363" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="1365" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="1367" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1369" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1371" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1373" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1375" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1377" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1379" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1381" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1383" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1385" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -4050,8 +4090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="C60" workbookViewId="0">
-      <selection activeCell="H65" sqref="H65"/>
+    <sheetView showRuler="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -6957,10 +6997,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D74"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -6970,7 +7010,7 @@
     <col min="3" max="16384" width="20.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -6983,8 +7023,11 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="20" customHeight="1">
+      <c r="E1" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="20" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -6997,8 +7040,11 @@
       <c r="D2" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="20" customHeight="1">
+      <c r="E2" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="20" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
@@ -7011,8 +7057,11 @@
       <c r="D3" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="20" customHeight="1">
+      <c r="E3" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="20" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>28</v>
       </c>
@@ -7025,8 +7074,11 @@
       <c r="D4" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="20" customHeight="1">
+      <c r="E4" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="20" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
@@ -7039,8 +7091,11 @@
       <c r="D5" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="20" customHeight="1">
+      <c r="E5" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="20" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>32</v>
       </c>
@@ -7053,8 +7108,11 @@
       <c r="D6" s="2">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="20" customHeight="1">
+      <c r="E6" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="20" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>34</v>
       </c>
@@ -7067,8 +7125,11 @@
       <c r="D7" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="20" customHeight="1">
+      <c r="E7" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="20" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>36</v>
       </c>
@@ -7081,8 +7142,11 @@
       <c r="D8" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="20" customHeight="1">
+      <c r="E8" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="20" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>38</v>
       </c>
@@ -7095,8 +7159,11 @@
       <c r="D9" s="2">
         <v>42</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="20" customHeight="1">
+      <c r="E9" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="20" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>40</v>
       </c>
@@ -7109,8 +7176,11 @@
       <c r="D10" s="2">
         <v>48</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="20" customHeight="1">
+      <c r="E10" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="20" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>42</v>
       </c>
@@ -7123,8 +7193,11 @@
       <c r="D11" s="2">
         <v>56</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="20" customHeight="1">
+      <c r="E11" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="20" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>44</v>
       </c>
@@ -7137,8 +7210,11 @@
       <c r="D12" s="2">
         <v>62</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="20" customHeight="1">
+      <c r="E12" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="20" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>46</v>
       </c>
@@ -7151,8 +7227,11 @@
       <c r="D13" s="2">
         <v>68</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="20" customHeight="1">
+      <c r="E13" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="20" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>48</v>
       </c>
@@ -7165,8 +7244,11 @@
       <c r="D14" s="2">
         <v>74</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="20" customHeight="1">
+      <c r="E14" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="20" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>50</v>
       </c>
@@ -7179,8 +7261,11 @@
       <c r="D15" s="2">
         <v>80</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="20" customHeight="1">
+      <c r="E15" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="20" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>51</v>
       </c>
@@ -7193,8 +7278,11 @@
       <c r="D16" s="2">
         <v>90</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="20" customHeight="1">
+      <c r="E16" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="20" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>52</v>
       </c>
@@ -7207,8 +7295,11 @@
       <c r="D17" s="2">
         <v>96</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="20" customHeight="1">
+      <c r="E17" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="20" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>53</v>
       </c>
@@ -7221,8 +7312,11 @@
       <c r="D18" s="2">
         <v>102</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="20" customHeight="1">
+      <c r="E18" s="2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="20" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>54</v>
       </c>
@@ -7235,8 +7329,11 @@
       <c r="D19" s="2">
         <v>108</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="20" customHeight="1">
+      <c r="E19" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="20" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>55</v>
       </c>
@@ -7249,8 +7346,11 @@
       <c r="D20" s="2">
         <v>114</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="20" customHeight="1">
+      <c r="E20" s="2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="20" customHeight="1">
       <c r="A21" s="2" t="s">
         <v>56</v>
       </c>
@@ -7262,6 +7362,9 @@
       </c>
       <c r="D21" s="2">
         <v>120</v>
+      </c>
+      <c r="E21" s="2">
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="20" customHeight="1">
@@ -7445,10 +7548,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -7457,7 +7560,7 @@
     <col min="3" max="16384" width="20.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -7470,8 +7573,11 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="20" customHeight="1">
+      <c r="E1" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="20" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -7484,8 +7590,11 @@
       <c r="D2" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="20" customHeight="1">
+      <c r="E2" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="20" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
@@ -7498,8 +7607,11 @@
       <c r="D3" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="20" customHeight="1">
+      <c r="E3" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="20" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
@@ -7512,8 +7624,11 @@
       <c r="D4" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="20" customHeight="1">
+      <c r="E4" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="20" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>29</v>
       </c>
@@ -7526,8 +7641,11 @@
       <c r="D5" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="20" customHeight="1">
+      <c r="E5" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="20" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
@@ -7540,8 +7658,11 @@
       <c r="D6" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="20" customHeight="1">
+      <c r="E6" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="20" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
@@ -7554,8 +7675,11 @@
       <c r="D7" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="20" customHeight="1">
+      <c r="E7" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="20" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>35</v>
       </c>
@@ -7568,8 +7692,11 @@
       <c r="D8" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="20" customHeight="1">
+      <c r="E8" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="20" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>37</v>
       </c>
@@ -7582,8 +7709,11 @@
       <c r="D9" s="2">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="20" customHeight="1">
+      <c r="E9" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="20" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>39</v>
       </c>
@@ -7596,8 +7726,11 @@
       <c r="D10" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="20" customHeight="1">
+      <c r="E10" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="20" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>41</v>
       </c>
@@ -7610,8 +7743,11 @@
       <c r="D11" s="2">
         <v>42</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="20" customHeight="1">
+      <c r="E11" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="20" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>43</v>
       </c>
@@ -7624,8 +7760,11 @@
       <c r="D12" s="2">
         <v>47</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="20" customHeight="1">
+      <c r="E12" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="20" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>45</v>
       </c>
@@ -7638,8 +7777,11 @@
       <c r="D13" s="2">
         <v>51</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="20" customHeight="1">
+      <c r="E13" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="20" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>47</v>
       </c>
@@ -7652,8 +7794,11 @@
       <c r="D14" s="2">
         <v>56</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="20" customHeight="1">
+      <c r="E14" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="20" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>49</v>
       </c>
@@ -7666,8 +7811,11 @@
       <c r="D15" s="2">
         <v>60</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="20" customHeight="1">
+      <c r="E15" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="20" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>51</v>
       </c>
@@ -7680,8 +7828,11 @@
       <c r="D16" s="2">
         <v>68</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="20" customHeight="1">
+      <c r="E16" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="20" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>52</v>
       </c>
@@ -7694,8 +7845,11 @@
       <c r="D17" s="2">
         <v>72</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="20" customHeight="1">
+      <c r="E17" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="20" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>53</v>
       </c>
@@ -7708,8 +7862,11 @@
       <c r="D18" s="2">
         <v>77</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="20" customHeight="1">
+      <c r="E18" s="2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="20" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>54</v>
       </c>
@@ -7722,8 +7879,11 @@
       <c r="D19" s="2">
         <v>81</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="20" customHeight="1">
+      <c r="E19" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="20" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>55</v>
       </c>
@@ -7736,8 +7896,11 @@
       <c r="D20" s="2">
         <v>86</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="20" customHeight="1">
+      <c r="E20" s="2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="20" customHeight="1">
       <c r="A21" s="2" t="s">
         <v>56</v>
       </c>
@@ -7750,38 +7913,41 @@
       <c r="D21" s="5">
         <v>90</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="20" customHeight="1">
+      <c r="E21" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="20" customHeight="1">
       <c r="B22" s="5"/>
     </row>
-    <row r="23" spans="1:4" ht="20" customHeight="1">
+    <row r="23" spans="1:5" ht="20" customHeight="1">
       <c r="B23" s="5"/>
     </row>
-    <row r="24" spans="1:4" ht="20" customHeight="1">
+    <row r="24" spans="1:5" ht="20" customHeight="1">
       <c r="B24" s="5"/>
     </row>
-    <row r="25" spans="1:4" ht="20" customHeight="1">
+    <row r="25" spans="1:5" ht="20" customHeight="1">
       <c r="B25" s="5"/>
     </row>
-    <row r="26" spans="1:4" ht="20" customHeight="1">
+    <row r="26" spans="1:5" ht="20" customHeight="1">
       <c r="B26" s="5"/>
     </row>
-    <row r="27" spans="1:4" ht="20" customHeight="1">
+    <row r="27" spans="1:5" ht="20" customHeight="1">
       <c r="B27" s="5"/>
     </row>
-    <row r="28" spans="1:4" ht="20" customHeight="1">
+    <row r="28" spans="1:5" ht="20" customHeight="1">
       <c r="B28" s="5"/>
     </row>
-    <row r="29" spans="1:4" ht="20" customHeight="1">
+    <row r="29" spans="1:5" ht="20" customHeight="1">
       <c r="B29" s="5"/>
     </row>
-    <row r="30" spans="1:4" ht="20" customHeight="1">
+    <row r="30" spans="1:5" ht="20" customHeight="1">
       <c r="B30" s="5"/>
     </row>
-    <row r="31" spans="1:4" ht="20" customHeight="1">
+    <row r="31" spans="1:5" ht="20" customHeight="1">
       <c r="B31" s="5"/>
     </row>
-    <row r="32" spans="1:4" ht="20" customHeight="1">
+    <row r="32" spans="1:5" ht="20" customHeight="1">
       <c r="B32" s="5"/>
     </row>
     <row r="33" spans="1:2" ht="20" customHeight="1">
@@ -8035,10 +8201,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -8047,7 +8213,7 @@
     <col min="3" max="16384" width="20.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -8060,8 +8226,11 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="20" customHeight="1">
+      <c r="E1" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="20" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -8074,8 +8243,11 @@
       <c r="D2" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="20" customHeight="1">
+      <c r="E2" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="20" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
@@ -8088,8 +8260,11 @@
       <c r="D3" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="20" customHeight="1">
+      <c r="E3" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="20" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
@@ -8102,8 +8277,11 @@
       <c r="D4" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="20" customHeight="1">
+      <c r="E4" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="20" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>29</v>
       </c>
@@ -8116,8 +8294,11 @@
       <c r="D5" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="20" customHeight="1">
+      <c r="E5" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="20" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
@@ -8130,8 +8311,11 @@
       <c r="D6" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="20" customHeight="1">
+      <c r="E6" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="20" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
@@ -8144,8 +8328,11 @@
       <c r="D7" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="20" customHeight="1">
+      <c r="E7" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="20" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>35</v>
       </c>
@@ -8158,8 +8345,11 @@
       <c r="D8" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="20" customHeight="1">
+      <c r="E8" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="20" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>37</v>
       </c>
@@ -8172,8 +8362,11 @@
       <c r="D9" s="2">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="20" customHeight="1">
+      <c r="E9" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="20" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>39</v>
       </c>
@@ -8186,8 +8379,11 @@
       <c r="D10" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="20" customHeight="1">
+      <c r="E10" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="20" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>41</v>
       </c>
@@ -8200,8 +8396,11 @@
       <c r="D11" s="2">
         <v>42</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="20" customHeight="1">
+      <c r="E11" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="20" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>43</v>
       </c>
@@ -8214,8 +8413,11 @@
       <c r="D12" s="2">
         <v>47</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="20" customHeight="1">
+      <c r="E12" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="20" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>45</v>
       </c>
@@ -8228,8 +8430,11 @@
       <c r="D13" s="2">
         <v>51</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="20" customHeight="1">
+      <c r="E13" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="20" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>47</v>
       </c>
@@ -8242,8 +8447,11 @@
       <c r="D14" s="2">
         <v>56</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="20" customHeight="1">
+      <c r="E14" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="20" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>49</v>
       </c>
@@ -8256,8 +8464,11 @@
       <c r="D15" s="2">
         <v>60</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="20" customHeight="1">
+      <c r="E15" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="20" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>51</v>
       </c>
@@ -8270,8 +8481,11 @@
       <c r="D16" s="2">
         <v>68</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="20" customHeight="1">
+      <c r="E16" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="20" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>52</v>
       </c>
@@ -8284,8 +8498,11 @@
       <c r="D17" s="2">
         <v>72</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="20" customHeight="1">
+      <c r="E17" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="20" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>53</v>
       </c>
@@ -8298,8 +8515,11 @@
       <c r="D18" s="2">
         <v>77</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="20" customHeight="1">
+      <c r="E18" s="2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="20" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>54</v>
       </c>
@@ -8312,8 +8532,11 @@
       <c r="D19" s="2">
         <v>81</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="20" customHeight="1">
+      <c r="E19" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="20" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>55</v>
       </c>
@@ -8326,8 +8549,11 @@
       <c r="D20" s="2">
         <v>86</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="20" customHeight="1">
+      <c r="E20" s="2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="20" customHeight="1">
       <c r="A21" s="2" t="s">
         <v>56</v>
       </c>
@@ -8340,56 +8566,59 @@
       <c r="D21" s="5">
         <v>90</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="20" customHeight="1">
+      <c r="E21" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="20" customHeight="1">
       <c r="B22" s="5"/>
     </row>
-    <row r="23" spans="1:4" ht="20" customHeight="1">
+    <row r="23" spans="1:5" ht="20" customHeight="1">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
     </row>
-    <row r="24" spans="1:4" ht="20" customHeight="1">
+    <row r="24" spans="1:5" ht="20" customHeight="1">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
     </row>
-    <row r="25" spans="1:4" ht="20" customHeight="1">
+    <row r="25" spans="1:5" ht="20" customHeight="1">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
     </row>
-    <row r="26" spans="1:4" ht="20" customHeight="1">
+    <row r="26" spans="1:5" ht="20" customHeight="1">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
     </row>
-    <row r="27" spans="1:4" ht="20" customHeight="1">
+    <row r="27" spans="1:5" ht="20" customHeight="1">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
     </row>
-    <row r="28" spans="1:4" ht="20" customHeight="1">
+    <row r="28" spans="1:5" ht="20" customHeight="1">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
     </row>
-    <row r="29" spans="1:4" ht="20" customHeight="1">
+    <row r="29" spans="1:5" ht="20" customHeight="1">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
     </row>
-    <row r="30" spans="1:4" ht="20" customHeight="1">
+    <row r="30" spans="1:5" ht="20" customHeight="1">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
     </row>
-    <row r="31" spans="1:4" ht="20" customHeight="1">
+    <row r="31" spans="1:5" ht="20" customHeight="1">
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
     </row>
-    <row r="32" spans="1:4" ht="20" customHeight="1">
+    <row r="32" spans="1:5" ht="20" customHeight="1">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -8785,10 +9014,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -8797,7 +9026,7 @@
     <col min="3" max="16384" width="20.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -8810,8 +9039,11 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="20" customHeight="1">
+      <c r="E1" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="20" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>27</v>
       </c>
@@ -8824,8 +9056,11 @@
       <c r="D2" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="20" customHeight="1">
+      <c r="E2" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="20" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
@@ -8838,8 +9073,11 @@
       <c r="D3" s="2">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="20" customHeight="1">
+      <c r="E3" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="20" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>31</v>
       </c>
@@ -8852,8 +9090,11 @@
       <c r="D4" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="20" customHeight="1">
+      <c r="E4" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="20" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
@@ -8866,8 +9107,11 @@
       <c r="D5" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="20" customHeight="1">
+      <c r="E5" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="20" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -8880,8 +9124,11 @@
       <c r="D6" s="2">
         <v>44</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="20" customHeight="1">
+      <c r="E6" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="20" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>37</v>
       </c>
@@ -8894,8 +9141,11 @@
       <c r="D7" s="2">
         <v>51</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="20" customHeight="1">
+      <c r="E7" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="20" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>39</v>
       </c>
@@ -8908,8 +9158,11 @@
       <c r="D8" s="2">
         <v>58</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="20" customHeight="1">
+      <c r="E8" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="20" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>41</v>
       </c>
@@ -8922,8 +9175,11 @@
       <c r="D9" s="2">
         <v>68</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="20" customHeight="1">
+      <c r="E9" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="20" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>43</v>
       </c>
@@ -8936,8 +9192,11 @@
       <c r="D10" s="2">
         <v>75</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="20" customHeight="1">
+      <c r="E10" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="20" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>45</v>
       </c>
@@ -8950,8 +9209,11 @@
       <c r="D11" s="2">
         <v>82</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="20" customHeight="1">
+      <c r="E11" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="20" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>47</v>
       </c>
@@ -8964,8 +9226,11 @@
       <c r="D12" s="2">
         <v>89</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="20" customHeight="1">
+      <c r="E12" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="20" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>49</v>
       </c>
@@ -8978,8 +9243,11 @@
       <c r="D13" s="2">
         <v>96</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="20" customHeight="1">
+      <c r="E13" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="20" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>51</v>
       </c>
@@ -8992,8 +9260,11 @@
       <c r="D14" s="2">
         <v>108</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="20" customHeight="1">
+      <c r="E14" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="20" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>52</v>
       </c>
@@ -9006,8 +9277,11 @@
       <c r="D15" s="2">
         <v>116</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="20" customHeight="1">
+      <c r="E15" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="20" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>53</v>
       </c>
@@ -9020,8 +9294,11 @@
       <c r="D16" s="2">
         <v>123</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="20" customHeight="1">
+      <c r="E16" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="20" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>54</v>
       </c>
@@ -9034,8 +9311,11 @@
       <c r="D17" s="2">
         <v>130</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="20" customHeight="1">
+      <c r="E17" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="20" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>55</v>
       </c>
@@ -9048,8 +9328,11 @@
       <c r="D18" s="2">
         <v>137</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="20" customHeight="1">
+      <c r="E18" s="2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="20" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>56</v>
       </c>
@@ -9062,38 +9345,41 @@
       <c r="D19" s="2">
         <v>144</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="20" customHeight="1">
+      <c r="E19" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="20" customHeight="1">
       <c r="B22" s="5"/>
     </row>
-    <row r="23" spans="1:4" ht="20" customHeight="1">
+    <row r="23" spans="1:5" ht="20" customHeight="1">
       <c r="B23" s="5"/>
     </row>
-    <row r="24" spans="1:4" ht="20" customHeight="1">
+    <row r="24" spans="1:5" ht="20" customHeight="1">
       <c r="B24" s="5"/>
     </row>
-    <row r="25" spans="1:4" ht="20" customHeight="1">
+    <row r="25" spans="1:5" ht="20" customHeight="1">
       <c r="B25" s="5"/>
     </row>
-    <row r="26" spans="1:4" ht="20" customHeight="1">
+    <row r="26" spans="1:5" ht="20" customHeight="1">
       <c r="B26" s="5"/>
     </row>
-    <row r="27" spans="1:4" ht="20" customHeight="1">
+    <row r="27" spans="1:5" ht="20" customHeight="1">
       <c r="B27" s="5"/>
     </row>
-    <row r="28" spans="1:4" ht="20" customHeight="1">
+    <row r="28" spans="1:5" ht="20" customHeight="1">
       <c r="B28" s="5"/>
     </row>
-    <row r="29" spans="1:4" ht="20" customHeight="1">
+    <row r="29" spans="1:5" ht="20" customHeight="1">
       <c r="B29" s="5"/>
     </row>
-    <row r="30" spans="1:4" ht="20" customHeight="1">
+    <row r="30" spans="1:5" ht="20" customHeight="1">
       <c r="B30" s="5"/>
     </row>
-    <row r="31" spans="1:4" ht="20" customHeight="1">
+    <row r="31" spans="1:5" ht="20" customHeight="1">
       <c r="B31" s="5"/>
     </row>
-    <row r="32" spans="1:4" ht="20" customHeight="1">
+    <row r="32" spans="1:5" ht="20" customHeight="1">
       <c r="B32" s="5"/>
     </row>
     <row r="33" spans="1:2" ht="20" customHeight="1">
@@ -9347,10 +9633,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -9361,7 +9647,7 @@
     <col min="5" max="16384" width="20.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -9374,8 +9660,11 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="20" customHeight="1">
+      <c r="E1" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="20" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>27</v>
       </c>
@@ -9388,8 +9677,11 @@
       <c r="D2" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="20" customHeight="1">
+      <c r="E2" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="20" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
@@ -9402,8 +9694,11 @@
       <c r="D3" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="20" customHeight="1">
+      <c r="E3" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="20" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>31</v>
       </c>
@@ -9416,8 +9711,11 @@
       <c r="D4" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="20" customHeight="1">
+      <c r="E4" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="20" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
@@ -9430,8 +9728,11 @@
       <c r="D5" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="20" customHeight="1">
+      <c r="E5" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="20" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -9444,8 +9745,11 @@
       <c r="D6" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="20" customHeight="1">
+      <c r="E6" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="20" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>37</v>
       </c>
@@ -9458,8 +9762,11 @@
       <c r="D7" s="2">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="20" customHeight="1">
+      <c r="E7" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="20" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>39</v>
       </c>
@@ -9472,8 +9779,11 @@
       <c r="D8" s="2">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="20" customHeight="1">
+      <c r="E8" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="20" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>41</v>
       </c>
@@ -9486,8 +9796,11 @@
       <c r="D9" s="2">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="20" customHeight="1">
+      <c r="E9" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="20" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>43</v>
       </c>
@@ -9500,8 +9813,11 @@
       <c r="D10" s="2">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="20" customHeight="1">
+      <c r="E10" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="20" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>45</v>
       </c>
@@ -9514,8 +9830,11 @@
       <c r="D11" s="2">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="20" customHeight="1">
+      <c r="E11" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="20" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>47</v>
       </c>
@@ -9528,8 +9847,11 @@
       <c r="D12" s="2">
         <v>37</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="20" customHeight="1">
+      <c r="E12" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="20" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>49</v>
       </c>
@@ -9542,8 +9864,11 @@
       <c r="D13" s="2">
         <v>40</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="20" customHeight="1">
+      <c r="E13" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="20" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>51</v>
       </c>
@@ -9556,8 +9881,11 @@
       <c r="D14" s="2">
         <v>45</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="20" customHeight="1">
+      <c r="E14" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="20" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>52</v>
       </c>
@@ -9570,8 +9898,11 @@
       <c r="D15" s="2">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="20" customHeight="1">
+      <c r="E15" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="20" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>53</v>
       </c>
@@ -9584,8 +9915,11 @@
       <c r="D16" s="2">
         <v>51</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="20" customHeight="1">
+      <c r="E16" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="20" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>54</v>
       </c>
@@ -9598,8 +9932,11 @@
       <c r="D17" s="2">
         <v>54</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="20" customHeight="1">
+      <c r="E17" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="20" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>55</v>
       </c>
@@ -9612,8 +9949,11 @@
       <c r="D18" s="2">
         <v>57</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="20" customHeight="1">
+      <c r="E18" s="2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="20" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>56</v>
       </c>
@@ -9626,38 +9966,41 @@
       <c r="D19" s="2">
         <v>60</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="20" customHeight="1">
+      <c r="E19" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="20" customHeight="1">
       <c r="B22" s="5"/>
     </row>
-    <row r="23" spans="1:4" ht="20" customHeight="1">
+    <row r="23" spans="1:5" ht="20" customHeight="1">
       <c r="B23" s="5"/>
     </row>
-    <row r="24" spans="1:4" ht="20" customHeight="1">
+    <row r="24" spans="1:5" ht="20" customHeight="1">
       <c r="B24" s="5"/>
     </row>
-    <row r="25" spans="1:4" ht="20" customHeight="1">
+    <row r="25" spans="1:5" ht="20" customHeight="1">
       <c r="B25" s="5"/>
     </row>
-    <row r="26" spans="1:4" ht="20" customHeight="1">
+    <row r="26" spans="1:5" ht="20" customHeight="1">
       <c r="B26" s="5"/>
     </row>
-    <row r="27" spans="1:4" ht="20" customHeight="1">
+    <row r="27" spans="1:5" ht="20" customHeight="1">
       <c r="B27" s="5"/>
     </row>
-    <row r="28" spans="1:4" ht="20" customHeight="1">
+    <row r="28" spans="1:5" ht="20" customHeight="1">
       <c r="B28" s="5"/>
     </row>
-    <row r="29" spans="1:4" ht="20" customHeight="1">
+    <row r="29" spans="1:5" ht="20" customHeight="1">
       <c r="B29" s="5"/>
     </row>
-    <row r="30" spans="1:4" ht="20" customHeight="1">
+    <row r="30" spans="1:5" ht="20" customHeight="1">
       <c r="B30" s="5"/>
     </row>
-    <row r="31" spans="1:4" ht="20" customHeight="1">
+    <row r="31" spans="1:5" ht="20" customHeight="1">
       <c r="B31" s="5"/>
     </row>
-    <row r="32" spans="1:4" ht="20" customHeight="1">
+    <row r="32" spans="1:5" ht="20" customHeight="1">
       <c r="B32" s="5"/>
     </row>
     <row r="33" spans="1:2" ht="20" customHeight="1">
@@ -9911,10 +10254,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -9923,7 +10266,7 @@
     <col min="3" max="16384" width="20.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -9936,8 +10279,11 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="20" customHeight="1">
+      <c r="E1" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="20" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>27</v>
       </c>
@@ -9950,8 +10296,11 @@
       <c r="D2" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="20" customHeight="1">
+      <c r="E2" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="20" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
@@ -9964,8 +10313,11 @@
       <c r="D3" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="20" customHeight="1">
+      <c r="E3" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="20" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>31</v>
       </c>
@@ -9978,8 +10330,11 @@
       <c r="D4" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="20" customHeight="1">
+      <c r="E4" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="20" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
@@ -9992,8 +10347,11 @@
       <c r="D5" s="2">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="20" customHeight="1">
+      <c r="E5" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="20" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -10006,8 +10364,11 @@
       <c r="D6" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="20" customHeight="1">
+      <c r="E6" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="20" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>37</v>
       </c>
@@ -10020,8 +10381,11 @@
       <c r="D7" s="2">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="20" customHeight="1">
+      <c r="E7" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="20" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>39</v>
       </c>
@@ -10034,8 +10398,11 @@
       <c r="D8" s="2">
         <v>39</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="20" customHeight="1">
+      <c r="E8" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="20" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>41</v>
       </c>
@@ -10048,8 +10415,11 @@
       <c r="D9" s="2">
         <v>45</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="20" customHeight="1">
+      <c r="E9" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="20" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>43</v>
       </c>
@@ -10062,8 +10432,11 @@
       <c r="D10" s="2">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="20" customHeight="1">
+      <c r="E10" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="20" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>45</v>
       </c>
@@ -10076,8 +10449,11 @@
       <c r="D11" s="2">
         <v>55</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="20" customHeight="1">
+      <c r="E11" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="20" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>47</v>
       </c>
@@ -10090,8 +10466,11 @@
       <c r="D12" s="2">
         <v>60</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="20" customHeight="1">
+      <c r="E12" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="20" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>49</v>
       </c>
@@ -10104,8 +10483,11 @@
       <c r="D13" s="2">
         <v>64</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="20" customHeight="1">
+      <c r="E13" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="20" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>51</v>
       </c>
@@ -10118,8 +10500,11 @@
       <c r="D14" s="2">
         <v>72</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="20" customHeight="1">
+      <c r="E14" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="20" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>52</v>
       </c>
@@ -10132,8 +10517,11 @@
       <c r="D15" s="2">
         <v>77</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="20" customHeight="1">
+      <c r="E15" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="20" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>53</v>
       </c>
@@ -10146,8 +10534,11 @@
       <c r="D16" s="2">
         <v>82</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="20" customHeight="1">
+      <c r="E16" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="20" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>54</v>
       </c>
@@ -10160,8 +10551,11 @@
       <c r="D17" s="2">
         <v>87</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="20" customHeight="1">
+      <c r="E17" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="20" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>55</v>
       </c>
@@ -10174,8 +10568,11 @@
       <c r="D18" s="2">
         <v>92</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="20" customHeight="1">
+      <c r="E18" s="2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="20" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>56</v>
       </c>
@@ -10188,62 +10585,65 @@
       <c r="D19" s="5">
         <v>96</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="20" customHeight="1">
+      <c r="E19" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="20" customHeight="1">
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
     </row>
-    <row r="22" spans="1:4" ht="20" customHeight="1">
+    <row r="22" spans="1:5" ht="20" customHeight="1">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
     </row>
-    <row r="23" spans="1:4" ht="20" customHeight="1">
+    <row r="23" spans="1:5" ht="20" customHeight="1">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
     </row>
-    <row r="24" spans="1:4" ht="20" customHeight="1">
+    <row r="24" spans="1:5" ht="20" customHeight="1">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
     </row>
-    <row r="25" spans="1:4" ht="20" customHeight="1">
+    <row r="25" spans="1:5" ht="20" customHeight="1">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
     </row>
-    <row r="26" spans="1:4" ht="20" customHeight="1">
+    <row r="26" spans="1:5" ht="20" customHeight="1">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
     </row>
-    <row r="27" spans="1:4" ht="20" customHeight="1">
+    <row r="27" spans="1:5" ht="20" customHeight="1">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
     </row>
-    <row r="28" spans="1:4" ht="20" customHeight="1">
+    <row r="28" spans="1:5" ht="20" customHeight="1">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
     </row>
-    <row r="29" spans="1:4" ht="20" customHeight="1">
+    <row r="29" spans="1:5" ht="20" customHeight="1">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
     </row>
-    <row r="30" spans="1:4" ht="20" customHeight="1">
+    <row r="30" spans="1:5" ht="20" customHeight="1">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
     </row>
-    <row r="31" spans="1:4" ht="20" customHeight="1">
+    <row r="31" spans="1:5" ht="20" customHeight="1">
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
     </row>
-    <row r="32" spans="1:4" ht="20" customHeight="1">
+    <row r="32" spans="1:5" ht="20" customHeight="1">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>

</xml_diff>